<commit_message>
:books: docs - Atualizando README.md
</commit_message>
<xml_diff>
--- a/dados/01_avaliacao_maturidade.xlsx
+++ b/dados/01_avaliacao_maturidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b755341190342fa/projetos/finops-automatic/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="11_F2F9792E8E9AF7F2F1F8744F2B5D2B7880D9490B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09857F2-E63E-4FAD-B333-EABE889CBDD7}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="11_F2F9792E8E9AF7F2F1F8744F2B5D2B7880D9490B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50799FBC-779F-49B6-8458-E7DACE4959CA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Domínio</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>Correr</t>
+  </si>
+  <si>
+    <t>✅ Processo consolidado e amplamente adotado pelas equipes. Revisão periódica garante conformidade.</t>
+  </si>
+  <si>
+    <t>🔄 Ferramentas ativas, mas ainda com uso limitado por áreas não técnicas. Treinamentos adicionais recomendados.</t>
+  </si>
+  <si>
+    <t>🚧 Processo ainda não implementado. Requer definição clara de centros de custo e critérios de rateio.</t>
+  </si>
+  <si>
+    <t>✅ Orçamentos previstos regularmente com base em tendências históricas. Forecast validado com stakeholders.</t>
+  </si>
+  <si>
+    <t>🔄 Estratégias aplicadas em parte da infraestrutura. Potencial de expansão com análise mais granular de workloads.</t>
+  </si>
+  <si>
+    <t>🚧 Não há rotina estabelecida para reavaliação de workloads. Sugere-se calendário de revisões trimestrais.</t>
+  </si>
+  <si>
+    <t>🔄 Reuniões realizadas com certa frequência, mas ainda com baixa participação intersetorial.</t>
+  </si>
+  <si>
+    <t>🚧 Ausência de visualizações centralizadas e acessíveis. Recomendado criar painel com métricas críticas (tags, budget, anomalias).</t>
   </si>
 </sst>
 </file>
@@ -560,7 +584,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
@@ -569,7 +593,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1562,7 +1586,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1570,7 +1594,7 @@
     <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.88671875" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -1601,7 +1625,9 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>23</v>
+      </c>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,9 +1638,11 @@
         <v>8</v>
       </c>
       <c r="C3" s="6">
-        <v>3</v>
-      </c>
-      <c r="D3" s="17"/>
+        <v>2</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1625,9 +1653,11 @@
         <v>10</v>
       </c>
       <c r="C4" s="6">
-        <v>3</v>
-      </c>
-      <c r="D4" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1640,7 +1670,9 @@
       <c r="C5" s="6">
         <v>3</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1653,7 +1685,9 @@
       <c r="C6" s="6">
         <v>2</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1666,7 +1700,9 @@
       <c r="C7" s="6">
         <v>1</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1679,7 +1715,9 @@
       <c r="C8" s="6">
         <v>2</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1692,7 +1730,9 @@
       <c r="C9" s="8">
         <v>1</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1783,7 +1823,7 @@
       </c>
       <c r="B3" s="10">
         <f>AVERAGEIF(Avaliação!$A$2:$A$9, A3, Avaliação!$C$2:$C$9)</f>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="C3" s="11" t="str">
         <f>IF(B3&lt;=1.4, "Rastejar", IF(B3&lt;=2.4, "Andar", "Correr"))</f>
@@ -1822,11 +1862,11 @@
       </c>
       <c r="B6" s="10">
         <f>AVERAGEIF(Avaliação!$A$2:$A$9, A6, Avaliação!$C$2:$C$9)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="11" t="str">
         <f>IF(B6&lt;=1.4, "Rastejar", IF(B6&lt;=2.4, "Andar", "Correr"))</f>
-        <v>Correr</v>
+        <v>Andar</v>
       </c>
     </row>
   </sheetData>

</xml_diff>